<commit_message>
Writing created account credential into test data while Account Resgistration Test
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\15-Sept-2023batch\opencart\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\java-eclipse-workspace\OpenCart\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3315BD60-ACC2-4D41-9A18-B0F87EEF7991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="17589" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="33120" windowHeight="17595"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>username</t>
   </si>
@@ -75,14 +74,24 @@
     <t>test@123</t>
   </si>
   <si>
-    <t>abc123@gmail.com</t>
+    <t>OZhgf@gmail.com</t>
+  </si>
+  <si>
+    <t>lNFvzmuv</t>
+  </si>
+  <si>
+    <t>OgGhu@gmail.com</t>
+  </si>
+  <si>
+    <t>bxXIwqhk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,45 +99,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="16"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -136,46 +116,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,97 +435,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884FCF78-0A3E-40BF-9E26-11C478AF56E2}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.23046875" customWidth="1"/>
-    <col min="2" max="2" width="17.3046875" customWidth="1"/>
-    <col min="3" max="3" width="18.15234375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.28515625"/>
+    <col min="2" max="2" customWidth="true" width="17.28515625"/>
+    <col min="3" max="3" customWidth="true" width="18.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s" s="0">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s" s="0">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s" s="0">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s" s="0">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{D3BE7519-95C3-4ACD-9AB4-5385C9508082}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{8456409A-CACC-4B7E-B78E-75E713148E0E}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{5E52A498-5B14-4BDC-BBF1-05425B8AC197}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{94E9D5A6-98A1-4A25-BDDE-C5B20EDA887E}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{968262D0-AE14-41EF-AB8A-08B3F886E797}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{75A4F8D6-7BF1-446B-9367-475FA4FB44C7}"/>
-    <hyperlink ref="B6" r:id="rId7" xr:uid="{01D5649A-5E55-45E1-9B81-1CE430C208A1}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>